<commit_message>
added some compoents to component select
</commit_message>
<xml_diff>
--- a/Electronics/Component_Selection.xlsx
+++ b/Electronics/Component_Selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gannon Bird\Documents\Git\ECE590_SeniorDesign\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC8D21F-0009-468C-BD1E-1601B03BBA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D7E0C1-4CDA-44DC-8FCC-4F21B9A86035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Part Number</t>
   </si>
@@ -75,16 +75,51 @@
   </si>
   <si>
     <t>Digikey Cost</t>
+  </si>
+  <si>
+    <t>ICM-20948</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>C726001</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>LPS22DFTR</t>
+  </si>
+  <si>
+    <t>Barometor</t>
+  </si>
+  <si>
+    <t>9-axis IMU/LOW G Acc</t>
+  </si>
+  <si>
+    <t>LPS22HHTR</t>
+  </si>
+  <si>
+    <t>C2827824</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,14 +145,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -396,16 +434,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.08984375" customWidth="1"/>
@@ -468,6 +506,271 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f>(I2)+IF(G2,7,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9.34</v>
+      </c>
+      <c r="E3" s="1">
+        <f>(D3*C3)</f>
+        <v>9.34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="J3" s="1">
+        <f>(I3)+IF(G3,7,0)</f>
+        <v>11.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="E4" s="1">
+        <f>(D4*C4)</f>
+        <v>3.95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <f>(I4)+IF(G4,7,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3.62</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E9" si="0">(D5*C5)</f>
+        <v>3.62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:J12" si="1">(I5)+IF(G5,7,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D10" s="1"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D15" s="1"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D16" s="1"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D17" s="1"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D18" s="1"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D19" s="1"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D20" s="1"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D21" s="1"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.35">
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed JLC extended part Fee
</commit_message>
<xml_diff>
--- a/Electronics/Component_Selection.xlsx
+++ b/Electronics/Component_Selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gannon Bird\Documents\Git\ECE590_SeniorDesign\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D7E0C1-4CDA-44DC-8FCC-4F21B9A86035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EC767C-0E79-4EC2-AC7E-34709B536B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,7 +516,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <f>(I2)+IF(G2,7,0)</f>
+        <f>(I2)+IF(G2,3,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -550,8 +550,8 @@
         <v>4.8600000000000003</v>
       </c>
       <c r="J3" s="1">
-        <f>(I3)+IF(G3,7,0)</f>
-        <v>11.86</v>
+        <f t="shared" ref="J3:J12" si="0">(I3)+IF(G3,3,0)</f>
+        <v>7.86</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <f>(I4)+IF(G4,7,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -602,7 +602,7 @@
         <v>3.62</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:E9" si="0">(D5*C5)</f>
+        <f t="shared" ref="E5:E9" si="1">(D5*C5)</f>
         <v>3.62</v>
       </c>
       <c r="F5" t="s">
@@ -618,55 +618,55 @@
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" ref="J5:J12" si="1">(I5)+IF(G5,7,0)</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D6" s="1"/>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D8" s="1"/>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D9" s="1"/>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -674,7 +674,7 @@
       <c r="D10" s="1"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -682,7 +682,7 @@
       <c r="D11" s="1"/>
       <c r="I11" s="2"/>
       <c r="J11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -690,7 +690,7 @@
       <c r="D12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
picked High G accelrometer
</commit_message>
<xml_diff>
--- a/Electronics/Component_Selection.xlsx
+++ b/Electronics/Component_Selection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gannon Bird\Documents\Git\ECE590_SeniorDesign\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894539BC-5086-40C1-A87B-5FF8EEDEC22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF67573-B86A-43D4-94C7-7B866987ECA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="8243" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Part Number</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>C97627</t>
+  </si>
+  <si>
+    <t>ADXL375BCCZ-RL7</t>
+  </si>
+  <si>
+    <t>High G Acc</t>
+  </si>
+  <si>
+    <t>C481898</t>
   </si>
 </sst>
 </file>
@@ -434,24 +443,24 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
-    <col min="6" max="6" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.06640625" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -517,7 +526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -551,7 +560,7 @@
         <v>7.86</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -585,19 +594,41 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.399999999999999</v>
+      </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E9" si="1">(D5*C5)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="2"/>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5.4210000000000003</v>
+      </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>8.4209999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D6" s="1"/>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
@@ -609,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D7" s="1"/>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
@@ -621,7 +652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D8" s="1"/>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
@@ -633,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D9" s="1"/>
       <c r="E9" s="1">
         <f t="shared" si="1"/>
@@ -645,7 +676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D10" s="1"/>
       <c r="I10" s="2"/>
       <c r="J10" s="1">
@@ -653,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D11" s="1"/>
       <c r="I11" s="2"/>
       <c r="J11" s="1">
@@ -661,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D12" s="1"/>
       <c r="I12" s="2"/>
       <c r="J12" s="1">
@@ -669,82 +700,82 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D13" s="1"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D14" s="1"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D15" s="1"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D16" s="1"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D17" s="1"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D18" s="1"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D19" s="1"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D20" s="1"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D21" s="1"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.45">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.45">
       <c r="D35" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kicad formating and others
</commit_message>
<xml_diff>
--- a/Electronics/Component_Selection.xlsx
+++ b/Electronics/Component_Selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gannon Bird\Documents\Git\ECE590_SeniorDesign\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E7C51E-4EC2-4F79-84BC-17D49EF4580A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F5E965-A0E3-42F9-807B-5FA0C99D2DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="0" windowWidth="14400" windowHeight="8243" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Part Number</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>C2613930</t>
+  </si>
+  <si>
+    <t>PKM13EPYH4000-A0</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
   </si>
 </sst>
 </file>
@@ -451,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -672,10 +678,30 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="D7" s="1"/>
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.41</v>
+      </c>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="1">

</xml_diff>